<commit_message>
update 08_position_subtype_HLA, fix subtype rank column
</commit_message>
<xml_diff>
--- a/08_position_subtype_HLA/subtype_HLA_regression_result.xlsx
+++ b/08_position_subtype_HLA/subtype_HLA_regression_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/202/hiv-capsid-data/08_position_subtype_HLA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA748FA7-354F-9A46-A18F-1CBBC40FBC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5154F5-32DB-0F46-B2D9-F79D9140F42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18860" yWindow="2620" windowWidth="41220" windowHeight="22540" xr2:uid="{068E35E1-2D64-824B-A245-3B8D84E36743}"/>
+    <workbookView xWindow="19420" yWindow="3820" windowWidth="41220" windowHeight="22540" xr2:uid="{068E35E1-2D64-824B-A245-3B8D84E36743}"/>
   </bookViews>
   <sheets>
     <sheet name="raw linear reg data" sheetId="2" r:id="rId1"/>
@@ -47,62 +47,6 @@
     <t>Subtype chi-square test and #HLA Reference with interaction, Rfit</t>
   </si>
   <si>
-    <t>## 
-## Call:
-## lm(formula = Entropy ~ subtype_rank + HLA, data = df)
-## 
-## Residuals:
-##      Min       1Q   Median       3Q      Max 
-## -0.63064 -0.12129  0.04776  0.04776  1.20449 
-## 
-## Coefficients:
-##               Estimate Std. Error t value Pr(&gt;|t|)    
-## (Intercept)  -0.050997   0.023846  -2.139   0.0335 *  
-## subtype_rank  0.001616   0.000244   6.622 2.51e-10 ***
-## HLA           0.116175   0.011516  10.088  &lt; 2e-16 ***
-## ---
-## Signif. codes:  0 '***' 0.001 '**' 0.01 '*' 0.05 '.' 0.1 ' ' 1
-## 
-## Residual standard error: 0.2477 on 228 degrees of freedom
-## Multiple R-squared:  0.6318, Adjusted R-squared:  0.6286 
-## F-statistic: 195.6 on 2 and 228 DF,  p-value: &lt; 2.2e-16</t>
-  </si>
-  <si>
-    <t>##                     2.5 %       97.5 %
-## (Intercept)  -0.097984402 -0.004009202
-## subtype_rank  0.001135112  0.002096718
-## HLA           0.093484362  0.138866266</t>
-  </si>
-  <si>
-    <t>## 
-## Call:
-## lm(formula = Entropy ~ subtype_rank * HLA, data = df)
-## 
-## Residuals:
-##      Min       1Q   Median       3Q      Max 
-## -0.57387 -0.12035  0.02421  0.02421  1.12006 
-## 
-## Coefficients:
-##                    Estimate Std. Error t value Pr(&gt;|t|)    
-## (Intercept)      -0.0273060  0.0190108  -1.436    0.152    
-## subtype_rank      0.0015486  0.0001935   8.003 6.22e-14 ***
-## HLA              -0.4757497  0.0515918  -9.221  &lt; 2e-16 ***
-## subtype_rank:HLA  0.0029941  0.0002568  11.657  &lt; 2e-16 ***
-## ---
-## Signif. codes:  0 '***' 0.001 '**' 0.01 '*' 0.05 '.' 0.1 ' ' 1
-## 
-## Residual standard error: 0.1963 on 227 degrees of freedom
-## Multiple R-squared:  0.7697, Adjusted R-squared:  0.7666 
-## F-statistic: 252.8 on 3 and 227 DF,  p-value: &lt; 2.2e-16</t>
-  </si>
-  <si>
-    <t>##                         2.5 %       97.5 %
-## (Intercept)      -0.064766143  0.010154241
-## subtype_rank      0.001167346  0.001929919
-## HLA              -0.577409861 -0.374089615
-## subtype_rank:HLA  0.002488011  0.003500237</t>
-  </si>
-  <si>
     <t>## Call:
 ## rfit.default(formula = Entropy ~ subtype + HLA, data = df)
 ## 
@@ -132,6 +76,62 @@
 ## 
 ## Multiple R-squared (Robust): 0.9320679 
 ## Reduction in Dispersion Test: 1038.191 p-value: 0</t>
+  </si>
+  <si>
+    <t>## 
+## Call:
+## lm(formula = Entropy ~ subtype_rank + HLA, data = df)
+## 
+## Residuals:
+##      Min       1Q   Median       3Q      Max 
+## -0.49054 -0.12676  0.05899  0.05899  1.08086 
+## 
+## Coefficients:
+##                Estimate Std. Error t value Pr(&gt;|t|)    
+## (Intercept)  -0.0649727  0.0179847  -3.613 0.000373 ***
+## subtype_rank  0.0059825  0.0004743  12.614  &lt; 2e-16 ***
+## HLA           0.0695970  0.0105914   6.571 3.35e-10 ***
+## ---
+## Signif. codes:  0 '***' 0.001 '**' 0.01 '*' 0.05 '.' 0.1 ' ' 1
+## 
+## Residual standard error: 0.2075 on 228 degrees of freedom
+## Multiple R-squared:  0.7414, Adjusted R-squared:  0.7391 
+## F-statistic: 326.8 on 2 and 228 DF,  p-value: &lt; 2.2e-16</t>
+  </si>
+  <si>
+    <t>##                     2.5 %       97.5 %
+## (Intercept)  -0.100410075 -0.029535301
+## subtype_rank  0.005047985  0.006917091
+## HLA           0.048727501  0.090466598</t>
+  </si>
+  <si>
+    <t>## 
+## Call:
+## lm(formula = Entropy ~ subtype_rank * HLA, data = df)
+## 
+## Residuals:
+##      Min       1Q   Median       3Q      Max 
+## -0.49577 -0.06789  0.02419  0.02419  1.05375 
+## 
+## Coefficients:
+##                    Estimate Std. Error t value Pr(&gt;|t|)    
+## (Intercept)      -0.0290519  0.0157400  -1.846   0.0662 .  
+## subtype_rank      0.0048617  0.0004199  11.578  &lt; 2e-16 ***
+## HLA              -0.1266590  0.0226494  -5.592 6.42e-08 ***
+## subtype_rank:HLA  0.0022689  0.0002403   9.441  &lt; 2e-16 ***
+## ---
+## Signif. codes:  0 '***' 0.001 '**' 0.01 '*' 0.05 '.' 0.1 ' ' 1
+## 
+## Residual standard error: 0.1763 on 227 degrees of freedom
+## Multiple R-squared:  0.8143, Adjusted R-squared:  0.8119 
+## F-statistic: 331.8 on 3 and 227 DF,  p-value: &lt; 2.2e-16</t>
+  </si>
+  <si>
+    <t>##                         2.5 %       97.5 %
+## (Intercept)      -0.060067012  0.001963226
+## subtype_rank      0.004034310  0.005689167
+## HLA              -0.171288986 -0.082028922
+## subtype_rank:HLA  0.001795338  0.002742393</t>
   </si>
 </sst>
 </file>
@@ -505,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61A72ED6-0FAD-B74E-89E2-B21629464E8A}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,18 +525,18 @@
     </row>
     <row r="2" spans="1:2" ht="360" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="90" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -549,10 +549,10 @@
     </row>
     <row r="7" spans="1:2" ht="252" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>